<commit_message>
additional changes for pop-up blocker
</commit_message>
<xml_diff>
--- a/data/webApp.SEOR.crm/crm_exportfile_xlsx.xlsx
+++ b/data/webApp.SEOR.crm/crm_exportfile_xlsx.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="124">
   <si>
     <t>Website</t>
   </si>
@@ -368,6 +368,30 @@
   </si>
   <si>
     <t>(183) 237-3390</t>
+  </si>
+  <si>
+    <t>glpu_230921102843_xlsx</t>
+  </si>
+  <si>
+    <t>glpu@gmail.com</t>
+  </si>
+  <si>
+    <t>http://www.zarnik.com</t>
+  </si>
+  <si>
+    <t>(880) 884-1256</t>
+  </si>
+  <si>
+    <t>wuxt_230921144044_xlsx</t>
+  </si>
+  <si>
+    <t>wuxt@gmail.com</t>
+  </si>
+  <si>
+    <t>https://raymooreservices.com</t>
+  </si>
+  <si>
+    <t>(472) 890-1929</t>
   </si>
 </sst>
 </file>
@@ -764,19 +788,19 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s" s="0">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>19</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>5</v>

</xml_diff>